<commit_message>
parameters for CACR & CAMD 2022
</commit_message>
<xml_diff>
--- a/parameters/Local/CACR-2022-Parameters.xlsx
+++ b/parameters/Local/CACR-2022-Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/xdevelopment/birding/automatingcbc/parameters/Local/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4CDE65-CC0F-3F4F-86FB-F8B0ACA6DB81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{317E7E68-5AD9-9443-A2DB-32C9B569CDEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35180" yWindow="5620" windowWidth="27320" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -937,7 +937,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B4" sqref="B4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -957,7 +957,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2">
-        <v>44913</v>
+        <v>44921</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>